<commit_message>
add lab 1 no videos yet
</commit_message>
<xml_diff>
--- a/vignettes/course_docs/Schedule_Spring.xlsx
+++ b/vignettes/course_docs/Schedule_Spring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattcrump/Github/psyc7709Lab/vignettes/course_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FB854A-777F-394C-BF68-BC927A9FDC65}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101A10BA-6F89-A74C-9534-2762EBB3BB21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="16220" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2300" yWindow="520" windowWidth="16220" windowHeight="14460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
update semester long project
</commit_message>
<xml_diff>
--- a/vignettes/course_docs/Schedule_Spring.xlsx
+++ b/vignettes/course_docs/Schedule_Spring.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattcrump/Github/psyc7709Lab/vignettes/course_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101A10BA-6F89-A74C-9534-2762EBB3BB21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80058929-0F46-2D49-AE9C-D9C6E85B08D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2300" yWindow="520" windowWidth="16220" windowHeight="14460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>Week</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>Kissing the cookie cutter goodbye</t>
+  </si>
+  <si>
+    <t>Semester Long Project 3</t>
   </si>
 </sst>
 </file>
@@ -459,7 +462,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -636,7 +639,7 @@
         <v>17</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
         <v>18</v>

</xml_diff>